<commit_message>
Fixed Owns method of ExcelBook - Fixed owns method ExcelBook not considering all types - Added extra alias methods for getCell
</commit_message>
<xml_diff>
--- a/tests/org.eclipse.epsilon.emc.cellsheet.excel.test/resources/Formula.xlsx
+++ b/tests/org.eclipse.epsilon.emc.cellsheet.excel.test/resources/Formula.xlsx
@@ -1,16 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10610"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C49910-4E6E-4E4C-87B2-220F22872B15}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90841868-8ECF-3240-A359-943785A8438A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Labels" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Formula" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,9 +22,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>This is another spreadsheet</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Eve</t>
+  </si>
+  <si>
+    <t>Label Ref</t>
+  </si>
+  <si>
+    <t>Label Ref Legacy</t>
+  </si>
+  <si>
+    <t>Label Ref Same Sheet</t>
+  </si>
+  <si>
+    <t>Label Ref Same Sheet Legacy</t>
   </si>
 </sst>
 </file>
@@ -340,15 +366,186 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7CA1A42-B638-E547-A921-2EE22C4EE037}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C07C3F92-35E2-774E-A2A7-D68AE94B1A7F}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="str">
+        <f>Labels!A1</f>
+        <v>Alice</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="str">
+        <f>+Labels!A1</f>
+        <v>Alice</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="str">
+        <f>A3</f>
+        <v>Label Ref Same Sheet</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="str">
+        <f>A4</f>
+        <v>Label Ref Same Sheet Legacy</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed getReferencedCells() for same sheet references - Added test for the above fix
</commit_message>
<xml_diff>
--- a/tests/org.eclipse.epsilon.emc.cellsheet.excel.test/resources/Formula.xlsx
+++ b/tests/org.eclipse.epsilon.emc.cellsheet.excel.test/resources/Formula.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10610"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8B6B8F-9585-4E46-BCA0-2FAA263CA8BF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B55290-42FA-1E46-B89B-385A25F28904}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Alice</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Sum region</t>
+  </si>
+  <si>
+    <t>Sum Region Same Sheet</t>
   </si>
 </sst>
 </file>
@@ -412,7 +415,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C19:C20"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -504,10 +507,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C07C3F92-35E2-774E-A2A7-D68AE94B1A7F}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -515,7 +518,7 @@
     <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -523,8 +526,14 @@
         <f>Labels!A1</f>
         <v>Alice</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="J1">
+        <v>1</v>
+      </c>
+      <c r="K1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -532,8 +541,14 @@
         <f>+Labels!A1</f>
         <v>Alice</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -541,8 +556,14 @@
         <f>A3</f>
         <v>Label Ref Same Sheet</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -550,14 +571,73 @@
         <f>A4</f>
         <v>Label Ref Same Sheet Legacy</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5">
         <f>SUM(Data!A1:B10)</f>
         <v>210</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <f>SUM(J1:K10)</f>
+        <v>210</v>
+      </c>
+      <c r="J6">
+        <v>6</v>
+      </c>
+      <c r="K6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <v>7</v>
+      </c>
+      <c r="K7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <v>8</v>
+      </c>
+      <c r="K8">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J9">
+        <v>9</v>
+      </c>
+      <c r="K9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J10">
+        <v>10</v>
+      </c>
+      <c r="K10">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>